<commit_message>
create tables and figures
</commit_message>
<xml_diff>
--- a/Output/Modelling/Logistic Regression/Tables/change_smote_model_comparison_df.xlsx
+++ b/Output/Modelling/Logistic Regression/Tables/change_smote_model_comparison_df.xlsx
@@ -490,20 +490,20 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0286</v>
+        <v>0.9472</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.0008</t>
+          <t>0.9097</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.0286</t>
+          <t>0.9472</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.0016</v>
+        <v>0.9281</v>
       </c>
     </row>
     <row r="4">
@@ -513,20 +513,20 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5984</v>
+        <v>0.9463</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9063</t>
+          <t>0.9096</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.5984</t>
+          <t>0.9463</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.7189</v>
+        <v>0.9276</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
change model table refresh
</commit_message>
<xml_diff>
--- a/Output/Modelling/Logistic Regression/Tables/change_smote_model_comparison_df.xlsx
+++ b/Output/Modelling/Logistic Regression/Tables/change_smote_model_comparison_df.xlsx
@@ -467,20 +467,20 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5742</v>
+        <v>0.5608</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.9115</t>
+          <t>0.9147</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.5742</t>
+          <t>0.5608</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.6961000000000001</v>
+        <v>0.6860000000000001</v>
       </c>
     </row>
     <row r="3">

</xml_diff>